<commit_message>
fixed historic data to give better weight estimations
</commit_message>
<xml_diff>
--- a/Data/RCAircraftHistoricWeightData.xlsx
+++ b/Data/RCAircraftHistoricWeightData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28926"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/48e263f47b741b0d/Documents/MATLAB/AAE451_SeniorDesign/Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nathe\Desktop\JZ-WannaBee\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{05B678EA-C071-416E-A507-CE039B5C5E95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44E75050-54F0-4056-85FD-1C8124B2B5A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Aircraft Data" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="382" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="378" uniqueCount="62">
   <si>
     <t>Source</t>
   </si>
@@ -162,9 +162,6 @@
   </si>
   <si>
     <t>JOANNEUM</t>
-  </si>
-  <si>
-    <t>ERAU</t>
   </si>
   <si>
     <t>SPITZFIRE</t>
@@ -234,7 +231,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -522,7 +519,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -577,7 +574,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:R48">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:R47">
   <tableColumns count="18">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Source"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Aircraft"/>
@@ -803,14 +800,14 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:R48"/>
+  <dimension ref="A1:R47"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H1" sqref="H1"/>
+      <selection pane="bottomLeft" activeCell="D51" sqref="D51"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="3" max="3" width="13.7109375" customWidth="1"/>
     <col min="4" max="4" width="14.28515625" customWidth="1"/>
@@ -827,7 +824,7 @@
     <col min="18" max="18" width="16.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="15.75" customHeight="1">
+    <row r="1" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -883,7 +880,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:18" ht="15.75" customHeight="1">
+    <row r="2" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="18"/>
       <c r="B2" s="19"/>
       <c r="C2" s="19"/>
@@ -903,7 +900,7 @@
       <c r="Q2" s="19"/>
       <c r="R2" s="20"/>
     </row>
-    <row r="3" spans="1:18" ht="15.75" customHeight="1">
+    <row r="3" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>18</v>
       </c>
@@ -959,7 +956,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:18" ht="15.75" customHeight="1">
+    <row r="4" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="9" t="s">
         <v>18</v>
       </c>
@@ -1015,7 +1012,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:18" ht="15.75" customHeight="1">
+    <row r="5" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
         <v>18</v>
       </c>
@@ -1071,7 +1068,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="1:18" ht="15.75" customHeight="1">
+    <row r="6" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="9" t="s">
         <v>18</v>
       </c>
@@ -1127,7 +1124,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:18" ht="15.75" customHeight="1">
+    <row r="7" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
         <v>18</v>
       </c>
@@ -1183,7 +1180,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="8" spans="1:18" ht="15.75" customHeight="1">
+    <row r="8" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="9" t="s">
         <v>18</v>
       </c>
@@ -1239,7 +1236,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="9" spans="1:18" ht="15.75" customHeight="1">
+    <row r="9" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
         <v>18</v>
       </c>
@@ -1295,7 +1292,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="10" spans="1:18" ht="15.75" customHeight="1">
+    <row r="10" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="9" t="s">
         <v>18</v>
       </c>
@@ -1351,7 +1348,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="11" spans="1:18" ht="15.75" customHeight="1">
+    <row r="11" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
         <v>18</v>
       </c>
@@ -1407,7 +1404,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="12" spans="1:18" ht="15.75" customHeight="1">
+    <row r="12" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="9" t="s">
         <v>18</v>
       </c>
@@ -1462,7 +1459,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="13" spans="1:18" ht="15.75" customHeight="1">
+    <row r="13" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
         <v>18</v>
       </c>
@@ -1517,7 +1514,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="14" spans="1:18" ht="15.75" customHeight="1">
+    <row r="14" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="9" t="s">
         <v>18</v>
       </c>
@@ -1572,7 +1569,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="15" spans="1:18" ht="15.75" customHeight="1">
+    <row r="15" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
         <v>18</v>
       </c>
@@ -1627,7 +1624,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="16" spans="1:18" ht="15.75" customHeight="1">
+    <row r="16" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="9" t="s">
         <v>18</v>
       </c>
@@ -1682,7 +1679,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="17" spans="1:18" ht="15.75" customHeight="1">
+    <row r="17" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="4" t="s">
         <v>18</v>
       </c>
@@ -1737,7 +1734,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="18" spans="1:18" ht="15.75" customHeight="1">
+    <row r="18" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="9" t="s">
         <v>18</v>
       </c>
@@ -1792,7 +1789,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="19" spans="1:18" ht="15.75" customHeight="1">
+    <row r="19" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="4" t="s">
         <v>18</v>
       </c>
@@ -1847,7 +1844,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="20" spans="1:18" ht="15.75" customHeight="1">
+    <row r="20" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="9" t="s">
         <v>18</v>
       </c>
@@ -1902,7 +1899,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="21" spans="1:18" ht="15.75" customHeight="1">
+    <row r="21" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="4" t="s">
         <v>18</v>
       </c>
@@ -1958,7 +1955,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="22" spans="1:18" ht="15.75" customHeight="1">
+    <row r="22" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="9" t="s">
         <v>18</v>
       </c>
@@ -2014,7 +2011,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="23" spans="1:18" ht="15.75" customHeight="1">
+    <row r="23" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="4" t="s">
         <v>18</v>
       </c>
@@ -2070,1364 +2067,1324 @@
         <v>25</v>
       </c>
     </row>
-    <row r="24" spans="1:18" ht="15.75" customHeight="1">
-      <c r="A24" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="B24" s="10"/>
-      <c r="C24" s="10" t="s">
+    <row r="24" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B24" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="D24" s="10">
+      <c r="C24" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="D24" s="5">
         <v>2022</v>
       </c>
-      <c r="E24" s="10">
+      <c r="E24" s="5">
+        <v>32</v>
+      </c>
+      <c r="F24" s="5">
+        <v>1</v>
+      </c>
+      <c r="G24" s="5">
+        <v>12.13</v>
+      </c>
+      <c r="H24" s="5">
+        <v>0</v>
+      </c>
+      <c r="I24" s="5">
+        <f t="shared" ref="I24:I29" si="3">G24-H24</f>
+        <v>12.13</v>
+      </c>
+      <c r="J24" s="5">
+        <v>1.59</v>
+      </c>
+      <c r="K24" s="6">
+        <f t="shared" ref="K24:K47" si="4">I24/G24</f>
+        <v>1</v>
+      </c>
+      <c r="L24" s="5"/>
+      <c r="M24" s="5"/>
+      <c r="N24" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="O24" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="P24" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q24" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="R24" s="8" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="25" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="B25" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="C25" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="D25" s="10">
+        <v>2022</v>
+      </c>
+      <c r="E25" s="10">
+        <v>32</v>
+      </c>
+      <c r="F25" s="10">
         <v>2</v>
       </c>
-      <c r="F24" s="10">
-        <v>2</v>
-      </c>
-      <c r="G24" s="10"/>
-      <c r="H24" s="10"/>
-      <c r="I24" s="10"/>
-      <c r="J24" s="10">
-        <v>1.4</v>
-      </c>
-      <c r="K24" s="10">
-        <v>0.44</v>
-      </c>
-      <c r="L24" s="10">
-        <v>0.21</v>
-      </c>
-      <c r="M24" s="10"/>
-      <c r="N24" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="O24" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="P24" s="10"/>
-      <c r="Q24" s="10"/>
-      <c r="R24" s="13"/>
-    </row>
-    <row r="25" spans="1:18" ht="15.75" customHeight="1">
-      <c r="A25" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="B25" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="C25" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="D25" s="5">
-        <v>2022</v>
-      </c>
-      <c r="E25" s="5">
-        <v>32</v>
-      </c>
-      <c r="F25" s="5">
-        <v>1</v>
-      </c>
-      <c r="G25" s="5">
-        <v>12.13</v>
-      </c>
-      <c r="H25" s="5">
-        <v>0</v>
-      </c>
-      <c r="I25" s="5">
-        <f t="shared" ref="I25:I30" si="3">G25-H25</f>
-        <v>12.13</v>
-      </c>
-      <c r="J25" s="5">
-        <v>1.59</v>
-      </c>
-      <c r="K25" s="6">
-        <f t="shared" ref="K25:K48" si="4">I25/G25</f>
-        <v>1</v>
-      </c>
-      <c r="L25" s="5"/>
-      <c r="M25" s="5"/>
-      <c r="N25" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="O25" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="P25" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="Q25" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="R25" s="8" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="26" spans="1:18" ht="15.75" customHeight="1">
-      <c r="A26" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="B26" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="C26" s="10" t="s">
-        <v>44</v>
-      </c>
-      <c r="D26" s="10">
-        <v>2022</v>
-      </c>
-      <c r="E26" s="10">
-        <v>32</v>
-      </c>
-      <c r="F26" s="10">
-        <v>2</v>
-      </c>
-      <c r="G26" s="10">
+      <c r="G25" s="10">
         <v>20.51</v>
       </c>
-      <c r="H26" s="10">
+      <c r="H25" s="10">
         <v>8.3800000000000008</v>
       </c>
-      <c r="I26" s="10">
+      <c r="I25" s="10">
         <f t="shared" si="3"/>
         <v>12.13</v>
       </c>
-      <c r="J26" s="10">
+      <c r="J25" s="10">
         <v>1.59</v>
       </c>
-      <c r="K26" s="11">
+      <c r="K25" s="11">
         <f t="shared" si="4"/>
         <v>0.59141882008776203</v>
       </c>
-      <c r="L26" s="10"/>
-      <c r="M26" s="10"/>
-      <c r="N26" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="O26" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="P26" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="Q26" s="10" t="s">
+      <c r="L25" s="10"/>
+      <c r="M25" s="10"/>
+      <c r="N25" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="O25" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="P25" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q25" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="R26" s="13" t="s">
+      <c r="R25" s="13" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="1:18" ht="15.75" customHeight="1">
-      <c r="A27" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="B27" s="5" t="s">
+    <row r="26" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B26" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="C26" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="C27" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="D27" s="5">
+      <c r="D26" s="5">
         <v>2022</v>
       </c>
-      <c r="E27" s="5">
+      <c r="E26" s="5">
         <v>32</v>
       </c>
-      <c r="F27" s="5">
+      <c r="F26" s="5">
         <v>3</v>
       </c>
-      <c r="G27" s="5">
+      <c r="G26" s="5">
         <v>16.13</v>
       </c>
-      <c r="H27" s="5">
+      <c r="H26" s="5">
         <v>4</v>
       </c>
-      <c r="I27" s="5">
+      <c r="I26" s="5">
         <f t="shared" si="3"/>
         <v>12.129999999999999</v>
       </c>
-      <c r="J27" s="5">
+      <c r="J26" s="5">
         <v>1.59</v>
       </c>
-      <c r="K27" s="6">
+      <c r="K26" s="6">
         <f t="shared" si="4"/>
         <v>0.75201487910725351</v>
       </c>
-      <c r="L27" s="5"/>
-      <c r="M27" s="5"/>
-      <c r="N27" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="O27" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="P27" s="5" t="s">
+      <c r="L26" s="5"/>
+      <c r="M26" s="5"/>
+      <c r="N26" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="O26" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="P26" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q26" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="R26" s="8" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="27" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="B27" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="Q27" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="R27" s="8" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="28" spans="1:18" ht="15.75" customHeight="1">
-      <c r="A28" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="B28" s="10" t="s">
+      <c r="C27" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="C28" s="10" t="s">
-        <v>47</v>
-      </c>
-      <c r="D28" s="10">
+      <c r="D27" s="10">
         <v>2022</v>
       </c>
-      <c r="E28" s="10">
+      <c r="E27" s="10">
         <v>11</v>
       </c>
-      <c r="F28" s="10">
+      <c r="F27" s="10">
         <v>1</v>
       </c>
-      <c r="G28" s="10">
+      <c r="G27" s="10">
         <v>12.52</v>
       </c>
-      <c r="H28" s="10">
+      <c r="H27" s="10">
         <v>0</v>
       </c>
-      <c r="I28" s="10">
+      <c r="I27" s="10">
         <f t="shared" si="3"/>
         <v>12.52</v>
       </c>
-      <c r="J28" s="10">
+      <c r="J27" s="10">
         <v>1.65</v>
       </c>
-      <c r="K28" s="11">
+      <c r="K27" s="11">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="L28" s="10"/>
-      <c r="M28" s="10">
+      <c r="L27" s="10"/>
+      <c r="M27" s="10">
         <v>71.2</v>
       </c>
-      <c r="N28" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="O28" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="P28" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="Q28" s="10" t="s">
+      <c r="N27" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="O27" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="P27" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q27" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="R28" s="13" t="s">
+      <c r="R27" s="13" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="29" spans="1:18" ht="12.6">
-      <c r="A29" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="B29" s="5" t="s">
+    <row r="28" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B28" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C28" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="C29" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="D29" s="5">
+      <c r="D28" s="5">
         <v>2022</v>
       </c>
-      <c r="E29" s="5">
+      <c r="E28" s="5">
         <v>11</v>
       </c>
-      <c r="F29" s="5">
+      <c r="F28" s="5">
         <v>2</v>
       </c>
-      <c r="G29" s="5">
+      <c r="G28" s="5">
         <v>14.2</v>
       </c>
-      <c r="H29" s="5">
+      <c r="H28" s="5">
         <v>1.62</v>
       </c>
-      <c r="I29" s="5">
+      <c r="I28" s="5">
         <f t="shared" si="3"/>
         <v>12.579999999999998</v>
       </c>
-      <c r="J29" s="5">
+      <c r="J28" s="5">
         <v>1.65</v>
       </c>
-      <c r="K29" s="6">
+      <c r="K28" s="6">
         <f t="shared" si="4"/>
         <v>0.88591549295774641</v>
       </c>
-      <c r="L29" s="5"/>
-      <c r="M29" s="5">
+      <c r="L28" s="5"/>
+      <c r="M28" s="5">
         <v>71.2</v>
       </c>
-      <c r="N29" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="O29" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="P29" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="Q29" s="5" t="s">
+      <c r="N28" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="O28" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="P28" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q28" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="R29" s="8" t="s">
+      <c r="R28" s="8" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="30" spans="1:18" ht="12.6">
-      <c r="A30" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="B30" s="10" t="s">
+    <row r="29" spans="1:18" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A29" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="B29" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="C29" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="C30" s="10" t="s">
-        <v>47</v>
-      </c>
-      <c r="D30" s="10">
+      <c r="D29" s="10">
         <v>2022</v>
       </c>
-      <c r="E30" s="10">
+      <c r="E29" s="10">
         <v>11</v>
       </c>
-      <c r="F30" s="10">
+      <c r="F29" s="10">
         <v>2</v>
       </c>
-      <c r="G30" s="10">
+      <c r="G29" s="10">
         <v>14.53</v>
       </c>
-      <c r="H30" s="10">
+      <c r="H29" s="10">
         <v>2.0299999999999998</v>
       </c>
-      <c r="I30" s="10">
+      <c r="I29" s="10">
         <f t="shared" si="3"/>
         <v>12.5</v>
       </c>
-      <c r="J30" s="10">
+      <c r="J29" s="10">
         <v>1.65</v>
       </c>
-      <c r="K30" s="11">
+      <c r="K29" s="11">
         <f t="shared" si="4"/>
         <v>0.86028905712319348</v>
       </c>
-      <c r="L30" s="10"/>
-      <c r="M30" s="10">
+      <c r="L29" s="10"/>
+      <c r="M29" s="10">
         <v>67.8</v>
       </c>
-      <c r="N30" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="O30" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="P30" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="Q30" s="10" t="s">
+      <c r="N29" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="O29" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="P29" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q29" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="R30" s="13" t="s">
+      <c r="R29" s="13" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="31" spans="1:18" ht="12.6">
-      <c r="A31" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="B31" s="5" t="s">
+    <row r="30" spans="1:18" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A30" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B30" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="C30" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="C31" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="D31" s="5">
+      <c r="D30" s="5">
         <v>2021</v>
       </c>
-      <c r="E31" s="5">
+      <c r="E30" s="5">
         <v>19</v>
       </c>
-      <c r="F31" s="5">
+      <c r="F30" s="5">
         <v>1</v>
       </c>
-      <c r="G31" s="5">
+      <c r="G30" s="5">
         <v>12.5</v>
       </c>
-      <c r="H31" s="5">
+      <c r="H30" s="5">
         <v>0</v>
       </c>
-      <c r="I31" s="5">
+      <c r="I30" s="5">
         <v>9.82</v>
       </c>
-      <c r="J31" s="5">
+      <c r="J30" s="5">
         <v>2.68</v>
       </c>
-      <c r="K31" s="6">
+      <c r="K30" s="6">
         <f t="shared" si="4"/>
         <v>0.78560000000000008</v>
       </c>
-      <c r="L31" s="5"/>
-      <c r="M31" s="5">
+      <c r="L30" s="5"/>
+      <c r="M30" s="5">
         <v>95.33</v>
       </c>
-      <c r="N31" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="O31" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="P31" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="Q31" s="5" t="s">
+      <c r="N30" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="O30" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="P30" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q30" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="R31" s="8" t="s">
+      <c r="R30" s="8" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="32" spans="1:18" ht="12.6">
-      <c r="A32" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="B32" s="10" t="s">
+    <row r="31" spans="1:18" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A31" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="B31" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="C31" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="C32" s="10" t="s">
-        <v>49</v>
-      </c>
-      <c r="D32" s="10">
+      <c r="D31" s="10">
         <v>2021</v>
       </c>
-      <c r="E32" s="10">
+      <c r="E31" s="10">
         <v>19</v>
       </c>
-      <c r="F32" s="10">
+      <c r="F31" s="10">
         <v>2</v>
       </c>
-      <c r="G32" s="10">
+      <c r="G31" s="10">
         <v>16.93</v>
       </c>
-      <c r="H32" s="10">
+      <c r="H31" s="10">
         <v>4.43</v>
       </c>
-      <c r="I32" s="10">
+      <c r="I31" s="10">
         <v>9.82</v>
       </c>
-      <c r="J32" s="10">
+      <c r="J31" s="10">
         <v>2.68</v>
       </c>
-      <c r="K32" s="11">
+      <c r="K31" s="11">
         <f t="shared" si="4"/>
         <v>0.58003544004725338</v>
       </c>
-      <c r="L32" s="10"/>
-      <c r="M32" s="10">
+      <c r="L31" s="10"/>
+      <c r="M31" s="10">
         <v>95.33</v>
       </c>
-      <c r="N32" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="O32" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="P32" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="Q32" s="10" t="s">
+      <c r="N31" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="O31" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="P31" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q31" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="R32" s="13" t="s">
+      <c r="R31" s="13" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="33" spans="1:18" ht="12.6">
-      <c r="A33" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="B33" s="5" t="s">
+    <row r="32" spans="1:18" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A32" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B32" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="C32" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="C33" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="D33" s="5">
+      <c r="D32" s="5">
         <v>2021</v>
       </c>
-      <c r="E33" s="5">
+      <c r="E32" s="5">
         <v>19</v>
       </c>
-      <c r="F33" s="5">
+      <c r="F32" s="5">
         <v>3</v>
       </c>
-      <c r="G33" s="5">
+      <c r="G32" s="5">
         <v>13.91</v>
       </c>
-      <c r="H33" s="5">
+      <c r="H32" s="5">
         <v>1.41</v>
       </c>
-      <c r="I33" s="5">
+      <c r="I32" s="5">
         <v>9.82</v>
       </c>
-      <c r="J33" s="5">
+      <c r="J32" s="5">
         <v>2.68</v>
       </c>
-      <c r="K33" s="6">
+      <c r="K32" s="6">
         <f t="shared" si="4"/>
         <v>0.70596693026599566</v>
       </c>
-      <c r="L33" s="5"/>
-      <c r="M33" s="5">
+      <c r="L32" s="5"/>
+      <c r="M32" s="5">
         <v>95.33</v>
       </c>
-      <c r="N33" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="O33" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="P33" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="Q33" s="5" t="s">
+      <c r="N32" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="O32" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="P32" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q32" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="R33" s="8" t="s">
+      <c r="R32" s="8" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="34" spans="1:18" ht="12.6">
-      <c r="A34" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="B34" s="10" t="s">
+    <row r="33" spans="1:18" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A33" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="B33" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="C33" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="C34" s="10" t="s">
-        <v>51</v>
-      </c>
-      <c r="D34" s="10">
+      <c r="D33" s="10">
         <v>2021</v>
       </c>
-      <c r="E34" s="10">
+      <c r="E33" s="10">
         <v>1</v>
       </c>
-      <c r="F34" s="10">
+      <c r="F33" s="10">
         <v>1</v>
       </c>
-      <c r="G34" s="10">
+      <c r="G33" s="10">
         <v>8.98</v>
       </c>
-      <c r="H34" s="10">
+      <c r="H33" s="10">
         <v>0</v>
       </c>
-      <c r="I34" s="10">
+      <c r="I33" s="10">
         <v>6.22</v>
       </c>
-      <c r="J34" s="10">
+      <c r="J33" s="10">
         <v>2.76</v>
       </c>
-      <c r="K34" s="11">
+      <c r="K33" s="11">
         <f t="shared" si="4"/>
         <v>0.69265033407572374</v>
       </c>
-      <c r="L34" s="10"/>
-      <c r="M34" s="10">
+      <c r="L33" s="10"/>
+      <c r="M33" s="10">
         <v>40.68</v>
       </c>
-      <c r="N34" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="O34" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="P34" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="Q34" s="10" t="s">
+      <c r="N33" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="O33" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="P33" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q33" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="R34" s="13" t="s">
+      <c r="R33" s="13" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="35" spans="1:18" ht="12.6">
-      <c r="A35" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="B35" s="5" t="s">
+    <row r="34" spans="1:18" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A34" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B34" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="C34" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="C35" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="D35" s="5">
+      <c r="D34" s="5">
         <v>2021</v>
       </c>
-      <c r="E35" s="5">
+      <c r="E34" s="5">
         <v>1</v>
       </c>
-      <c r="F35" s="5">
+      <c r="F34" s="5">
         <v>2</v>
       </c>
-      <c r="G35" s="5">
+      <c r="G34" s="5">
         <v>18.239999999999998</v>
       </c>
-      <c r="H35" s="5">
+      <c r="H34" s="5">
         <v>9.26</v>
       </c>
-      <c r="I35" s="5">
+      <c r="I34" s="5">
         <v>6.22</v>
       </c>
-      <c r="J35" s="5">
+      <c r="J34" s="5">
         <v>2.76</v>
       </c>
-      <c r="K35" s="6">
+      <c r="K34" s="6">
         <f t="shared" si="4"/>
         <v>0.34100877192982459</v>
       </c>
-      <c r="L35" s="5"/>
-      <c r="M35" s="5">
+      <c r="L34" s="5"/>
+      <c r="M34" s="5">
         <v>58.01</v>
       </c>
-      <c r="N35" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="O35" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="P35" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="Q35" s="5" t="s">
+      <c r="N34" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="O34" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="P34" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q34" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="R35" s="8" t="s">
+      <c r="R34" s="8" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="36" spans="1:18" ht="12.6">
-      <c r="A36" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="B36" s="10" t="s">
+    <row r="35" spans="1:18" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A35" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="B35" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="C35" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="C36" s="10" t="s">
-        <v>51</v>
-      </c>
-      <c r="D36" s="10">
+      <c r="D35" s="10">
         <v>2021</v>
       </c>
-      <c r="E36" s="10">
+      <c r="E35" s="10">
         <v>1</v>
       </c>
-      <c r="F36" s="10">
+      <c r="F35" s="10">
         <v>3</v>
       </c>
-      <c r="G36" s="10">
+      <c r="G35" s="10">
         <v>9.73</v>
       </c>
-      <c r="H36" s="10">
+      <c r="H35" s="10">
         <v>0.75</v>
       </c>
-      <c r="I36" s="10">
+      <c r="I35" s="10">
         <v>6.22</v>
       </c>
-      <c r="J36" s="10">
+      <c r="J35" s="10">
         <v>2.76</v>
       </c>
-      <c r="K36" s="11">
+      <c r="K35" s="11">
         <f t="shared" si="4"/>
         <v>0.63926002055498454</v>
       </c>
-      <c r="L36" s="10"/>
-      <c r="M36" s="10">
+      <c r="L35" s="10"/>
+      <c r="M35" s="10">
         <v>42.52</v>
       </c>
-      <c r="N36" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="O36" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="P36" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="Q36" s="10" t="s">
+      <c r="N35" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="O35" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="P35" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q35" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="R36" s="13" t="s">
+      <c r="R35" s="13" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="37" spans="1:18" ht="12.6">
-      <c r="A37" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="B37" s="5" t="s">
+    <row r="36" spans="1:18" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A36" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B36" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="C36" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="C37" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="D37" s="5">
+      <c r="D36" s="5">
         <v>2021</v>
       </c>
-      <c r="E37" s="5">
+      <c r="E36" s="5">
         <v>2</v>
       </c>
-      <c r="F37" s="5">
+      <c r="F36" s="5">
         <v>1</v>
       </c>
-      <c r="G37" s="5">
+      <c r="G36" s="5">
         <v>6.3410000000000002</v>
       </c>
-      <c r="H37" s="5">
+      <c r="H36" s="5">
         <v>9.7000000000000003E-2</v>
       </c>
-      <c r="I37" s="5">
+      <c r="I36" s="5">
         <v>5.4279999999999999</v>
       </c>
-      <c r="J37" s="5">
+      <c r="J36" s="5">
         <v>0.81599999999999995</v>
       </c>
-      <c r="K37" s="6">
+      <c r="K36" s="6">
         <f t="shared" si="4"/>
         <v>0.85601640119854905</v>
       </c>
-      <c r="L37" s="5"/>
-      <c r="M37" s="5">
+      <c r="L36" s="5"/>
+      <c r="M36" s="5">
         <v>82.074667000000005</v>
       </c>
-      <c r="N37" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="O37" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="P37" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="Q37" s="5" t="s">
+      <c r="N36" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="O36" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="P36" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q36" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="R37" s="8" t="s">
+      <c r="R36" s="8" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="38" spans="1:18" ht="12.6">
-      <c r="A38" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="B38" s="10" t="s">
+    <row r="37" spans="1:18" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A37" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="B37" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="C37" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="C38" s="10" t="s">
-        <v>53</v>
-      </c>
-      <c r="D38" s="10">
+      <c r="D37" s="10">
         <v>2021</v>
       </c>
-      <c r="E38" s="10">
+      <c r="E37" s="10">
         <v>2</v>
       </c>
-      <c r="F38" s="10">
+      <c r="F37" s="10">
         <v>2</v>
       </c>
-      <c r="G38" s="10">
+      <c r="G37" s="10">
         <v>12.699</v>
       </c>
-      <c r="H38" s="10">
+      <c r="H37" s="10">
         <v>6.4550000000000001</v>
       </c>
-      <c r="I38" s="10">
+      <c r="I37" s="10">
         <v>5.4279999999999999</v>
       </c>
-      <c r="J38" s="10">
+      <c r="J37" s="10">
         <v>0.81599999999999995</v>
       </c>
-      <c r="K38" s="11">
+      <c r="K37" s="11">
         <f t="shared" si="4"/>
         <v>0.4274352311205607</v>
       </c>
-      <c r="L38" s="10"/>
-      <c r="M38" s="10">
+      <c r="L37" s="10"/>
+      <c r="M37" s="10">
         <v>73.861333000000002</v>
       </c>
-      <c r="N38" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="O38" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="P38" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="Q38" s="10" t="s">
+      <c r="N37" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="O37" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="P37" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q37" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="R38" s="13" t="s">
+      <c r="R37" s="13" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="39" spans="1:18" ht="12.6">
-      <c r="A39" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="B39" s="5" t="s">
+    <row r="38" spans="1:18" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A38" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B38" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="C38" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="C39" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="D39" s="5">
+      <c r="D38" s="5">
         <v>2021</v>
       </c>
-      <c r="E39" s="5">
+      <c r="E38" s="5">
         <v>2</v>
       </c>
-      <c r="F39" s="5">
+      <c r="F38" s="5">
         <v>3</v>
       </c>
-      <c r="G39" s="5">
+      <c r="G38" s="5">
         <v>10.057</v>
       </c>
-      <c r="H39" s="5">
+      <c r="H38" s="5">
         <v>2.9969999999999999</v>
       </c>
-      <c r="I39" s="5">
+      <c r="I38" s="5">
         <v>5.4279999999999999</v>
       </c>
-      <c r="J39" s="5">
+      <c r="J38" s="5">
         <v>1.6319999999999999</v>
       </c>
-      <c r="K39" s="6">
+      <c r="K38" s="6">
         <f t="shared" si="4"/>
         <v>0.53972357561897188</v>
       </c>
-      <c r="L39" s="5"/>
-      <c r="M39" s="5">
+      <c r="L38" s="5"/>
+      <c r="M38" s="5">
         <v>68.141333000000003</v>
       </c>
-      <c r="N39" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="O39" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="P39" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="Q39" s="5" t="s">
+      <c r="N38" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="O38" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="P38" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q38" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="R39" s="8" t="s">
+      <c r="R38" s="8" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="40" spans="1:18" ht="12.6">
-      <c r="A40" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="B40" s="10" t="s">
-        <v>54</v>
-      </c>
-      <c r="C40" s="10" t="s">
+    <row r="39" spans="1:18" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A39" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="B39" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="C39" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="D40" s="10">
+      <c r="D39" s="10">
         <v>2020</v>
       </c>
-      <c r="E40" s="10">
+      <c r="E39" s="10">
         <v>1</v>
       </c>
-      <c r="F40" s="10">
+      <c r="F39" s="10">
         <v>1</v>
       </c>
-      <c r="G40" s="10">
+      <c r="G39" s="10">
         <v>6.4</v>
       </c>
-      <c r="H40" s="10">
+      <c r="H39" s="10">
         <v>0</v>
       </c>
-      <c r="I40" s="10">
+      <c r="I39" s="10">
         <v>4.9000000000000004</v>
       </c>
-      <c r="J40" s="10">
+      <c r="J39" s="10">
         <v>1.5</v>
       </c>
-      <c r="K40" s="11">
+      <c r="K39" s="11">
         <f t="shared" si="4"/>
         <v>0.765625</v>
       </c>
-      <c r="L40" s="10"/>
-      <c r="M40" s="10">
+      <c r="L39" s="10"/>
+      <c r="M39" s="10">
         <v>71</v>
       </c>
-      <c r="N40" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="O40" s="10" t="s">
-        <v>55</v>
-      </c>
-      <c r="P40" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="Q40" s="10" t="s">
+      <c r="N39" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="O39" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="P39" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q39" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="R40" s="13" t="s">
+      <c r="R39" s="13" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="41" spans="1:18" ht="12.6">
-      <c r="A41" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="B41" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="C41" s="5" t="s">
+    <row r="40" spans="1:18" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A40" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B40" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="C40" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="D41" s="5">
+      <c r="D40" s="5">
         <v>2020</v>
       </c>
-      <c r="E41" s="5">
+      <c r="E40" s="5">
         <v>1</v>
       </c>
-      <c r="F41" s="5">
+      <c r="F40" s="5">
         <v>2</v>
       </c>
-      <c r="G41" s="5">
+      <c r="G40" s="5">
         <v>24</v>
       </c>
-      <c r="H41" s="5">
+      <c r="H40" s="5">
         <v>15.4</v>
       </c>
-      <c r="I41" s="5">
+      <c r="I40" s="5">
         <v>4.9000000000000004</v>
       </c>
-      <c r="J41" s="5">
+      <c r="J40" s="5">
         <v>1.5</v>
       </c>
-      <c r="K41" s="6">
+      <c r="K40" s="6">
         <f t="shared" si="4"/>
         <v>0.20416666666666669</v>
       </c>
-      <c r="L41" s="5"/>
-      <c r="M41" s="5">
+      <c r="L40" s="5"/>
+      <c r="M40" s="5">
         <v>165</v>
       </c>
-      <c r="N41" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="O41" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="P41" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="Q41" s="5" t="s">
+      <c r="N40" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="O40" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="P40" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q40" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="R41" s="8" t="s">
+      <c r="R40" s="8" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="42" spans="1:18" ht="12.6">
-      <c r="A42" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="B42" s="10" t="s">
-        <v>54</v>
-      </c>
-      <c r="C42" s="10" t="s">
+    <row r="41" spans="1:18" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A41" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="B41" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="C41" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="D42" s="10">
+      <c r="D41" s="10">
         <v>2020</v>
       </c>
-      <c r="E42" s="10">
+      <c r="E41" s="10">
         <v>1</v>
       </c>
-      <c r="F42" s="10">
+      <c r="F41" s="10">
         <v>3</v>
       </c>
-      <c r="G42" s="10">
+      <c r="G41" s="10">
         <v>9.4</v>
       </c>
-      <c r="H42" s="10">
+      <c r="H41" s="10">
         <v>1.6</v>
       </c>
-      <c r="I42" s="10">
+      <c r="I41" s="10">
         <v>4.9000000000000004</v>
       </c>
-      <c r="J42" s="10">
+      <c r="J41" s="10">
         <v>2.9</v>
       </c>
-      <c r="K42" s="11">
+      <c r="K41" s="11">
         <f t="shared" si="4"/>
         <v>0.52127659574468088</v>
       </c>
-      <c r="L42" s="10"/>
-      <c r="M42" s="10">
+      <c r="L41" s="10"/>
+      <c r="M41" s="10">
         <v>45</v>
       </c>
-      <c r="N42" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="O42" s="10" t="s">
+      <c r="N41" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="O41" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="P41" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q41" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="R41" s="13" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="42" spans="1:18" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A42" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B42" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="P42" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="Q42" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="R42" s="13" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="43" spans="1:18" ht="12.6">
-      <c r="A43" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="B43" s="5" t="s">
+      <c r="C42" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="C43" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="D43" s="5">
+      <c r="D42" s="5">
         <v>2020</v>
       </c>
-      <c r="E43" s="5">
+      <c r="E42" s="5">
         <v>2</v>
       </c>
-      <c r="F43" s="5">
+      <c r="F42" s="5">
         <v>1</v>
       </c>
-      <c r="G43" s="5">
+      <c r="G42" s="5">
         <v>8.3000000000000007</v>
       </c>
-      <c r="H43" s="5">
+      <c r="H42" s="5">
         <v>0</v>
       </c>
-      <c r="I43" s="5">
+      <c r="I42" s="5">
         <v>6.57</v>
       </c>
-      <c r="J43" s="5">
+      <c r="J42" s="5">
         <v>1.7</v>
       </c>
-      <c r="K43" s="6">
+      <c r="K42" s="6">
         <f t="shared" si="4"/>
         <v>0.79156626506024097</v>
       </c>
-      <c r="L43" s="5"/>
-      <c r="M43" s="5">
+      <c r="L42" s="5"/>
+      <c r="M42" s="5">
         <v>123</v>
       </c>
-      <c r="N43" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="O43" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="P43" s="5" t="s">
+      <c r="N42" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="O42" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="P42" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="Q43" s="5" t="s">
+      <c r="Q42" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="R43" s="8" t="s">
+      <c r="R42" s="8" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="44" spans="1:18" ht="12.6">
-      <c r="A44" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="B44" s="10" t="s">
+    <row r="43" spans="1:18" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A43" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="B43" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="C43" s="10" t="s">
         <v>56</v>
       </c>
-      <c r="C44" s="10" t="s">
-        <v>57</v>
-      </c>
-      <c r="D44" s="10">
+      <c r="D43" s="10">
         <v>2020</v>
       </c>
-      <c r="E44" s="10">
+      <c r="E43" s="10">
         <v>2</v>
       </c>
-      <c r="F44" s="10">
+      <c r="F43" s="10">
         <v>2</v>
       </c>
-      <c r="G44" s="10">
+      <c r="G43" s="10">
         <v>20.7</v>
       </c>
-      <c r="H44" s="10">
+      <c r="H43" s="10">
         <v>12.5</v>
       </c>
-      <c r="I44" s="10">
+      <c r="I43" s="10">
         <v>6.57</v>
       </c>
-      <c r="J44" s="10">
+      <c r="J43" s="10">
         <v>1.7</v>
       </c>
-      <c r="K44" s="11">
+      <c r="K43" s="11">
         <f t="shared" si="4"/>
         <v>0.31739130434782609</v>
       </c>
-      <c r="L44" s="10"/>
-      <c r="M44" s="10">
+      <c r="L43" s="10"/>
+      <c r="M43" s="10">
         <v>121</v>
       </c>
-      <c r="N44" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="O44" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="P44" s="10" t="s">
+      <c r="N43" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="O43" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="P43" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="Q44" s="10" t="s">
+      <c r="Q43" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="R44" s="13" t="s">
+      <c r="R43" s="13" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="45" spans="1:18" ht="12.6">
-      <c r="A45" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="B45" s="5" t="s">
+    <row r="44" spans="1:18" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A44" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B44" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="C44" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="C45" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="D45" s="5">
+      <c r="D44" s="5">
         <v>2020</v>
       </c>
-      <c r="E45" s="5">
+      <c r="E44" s="5">
         <v>2</v>
       </c>
-      <c r="F45" s="5">
+      <c r="F44" s="5">
         <v>3</v>
       </c>
-      <c r="G45" s="5">
+      <c r="G44" s="5">
         <v>10.9</v>
       </c>
-      <c r="H45" s="5">
+      <c r="H44" s="5">
         <v>0.91</v>
       </c>
-      <c r="I45" s="5">
+      <c r="I44" s="5">
         <v>6.57</v>
       </c>
-      <c r="J45" s="5">
+      <c r="J44" s="5">
         <v>3.4</v>
       </c>
-      <c r="K45" s="6">
+      <c r="K44" s="6">
         <f t="shared" si="4"/>
         <v>0.60275229357798166</v>
       </c>
-      <c r="L45" s="5"/>
-      <c r="M45" s="5">
+      <c r="L44" s="5"/>
+      <c r="M44" s="5">
         <v>48</v>
       </c>
-      <c r="N45" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="O45" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="P45" s="5" t="s">
+      <c r="N44" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="O44" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="P44" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="Q45" s="5" t="s">
+      <c r="Q44" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="R45" s="8" t="s">
+      <c r="R44" s="8" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="46" spans="1:18" ht="12.6">
-      <c r="A46" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="B46" s="10" t="s">
+    <row r="45" spans="1:18" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A45" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="B45" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="C45" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="C46" s="10" t="s">
-        <v>59</v>
-      </c>
-      <c r="D46" s="10">
+      <c r="D45" s="10">
         <v>2017</v>
       </c>
-      <c r="E46" s="10">
+      <c r="E45" s="10">
         <v>1</v>
       </c>
-      <c r="F46" s="10">
+      <c r="F45" s="10">
         <v>1</v>
       </c>
-      <c r="G46" s="10">
+      <c r="G45" s="10">
         <v>691</v>
       </c>
-      <c r="H46" s="10">
+      <c r="H45" s="10">
         <v>0</v>
       </c>
-      <c r="I46" s="10">
+      <c r="I45" s="10">
         <v>461</v>
       </c>
-      <c r="J46" s="10">
+      <c r="J45" s="10">
         <v>1.5</v>
       </c>
-      <c r="K46" s="11">
+      <c r="K45" s="11">
         <f t="shared" si="4"/>
         <v>0.66714905933429813</v>
       </c>
-      <c r="L46" s="10"/>
-      <c r="M46" s="10">
-        <v>23</v>
-      </c>
-      <c r="N46" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="O46" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="P46" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="Q46" s="10" t="s">
+      <c r="L45" s="10"/>
+      <c r="M45" s="10">
+        <v>23</v>
+      </c>
+      <c r="N45" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="O45" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="P45" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q45" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="R46" s="13" t="s">
+      <c r="R45" s="13" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="47" spans="1:18" ht="12.6">
-      <c r="A47" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="B47" s="5" t="s">
+    <row r="46" spans="1:18" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A46" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B46" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="C46" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="C47" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="D47" s="5">
+      <c r="D46" s="5">
         <v>2016</v>
       </c>
-      <c r="E47" s="5">
+      <c r="E46" s="5">
         <v>1</v>
       </c>
-      <c r="F47" s="5">
+      <c r="F46" s="5">
         <v>1</v>
       </c>
-      <c r="G47" s="5">
+      <c r="G46" s="5">
         <v>3.6469999999999998</v>
       </c>
-      <c r="H47" s="5">
+      <c r="H46" s="5">
         <v>2</v>
       </c>
-      <c r="I47" s="5">
-        <f>G47-H47</f>
+      <c r="I46" s="5">
+        <f>G46-H46</f>
         <v>1.6469999999999998</v>
       </c>
-      <c r="J47" s="5">
+      <c r="J46" s="5">
         <v>0.32400000000000001</v>
       </c>
-      <c r="K47" s="6">
+      <c r="K46" s="6">
         <f t="shared" si="4"/>
         <v>0.45160405812996979</v>
       </c>
-      <c r="L47" s="5"/>
-      <c r="M47" s="5">
+      <c r="L46" s="5"/>
+      <c r="M46" s="5">
         <v>70</v>
       </c>
-      <c r="N47" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="O47" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="P47" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="Q47" s="5" t="s">
+      <c r="N46" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="O46" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="P46" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q46" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="R47" s="8" t="s">
+      <c r="R46" s="8" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="48" spans="1:18" ht="15.75" customHeight="1">
-      <c r="A48" s="14" t="s">
-        <v>18</v>
-      </c>
-      <c r="B48" s="15" t="s">
-        <v>62</v>
-      </c>
-      <c r="C48" s="15" t="s">
+    <row r="47" spans="1:18" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A47" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="B47" s="15" t="s">
+        <v>61</v>
+      </c>
+      <c r="C47" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="D48" s="15">
+      <c r="D47" s="15">
         <v>2015</v>
       </c>
-      <c r="E48" s="15">
+      <c r="E47" s="15">
         <v>1</v>
       </c>
-      <c r="F48" s="15">
+      <c r="F47" s="15">
         <v>2</v>
       </c>
-      <c r="G48" s="15">
+      <c r="G47" s="15">
         <v>7.87</v>
       </c>
-      <c r="H48" s="15">
+      <c r="H47" s="15">
         <v>5.0049999999999999</v>
       </c>
-      <c r="I48" s="15">
+      <c r="I47" s="15">
         <v>2.8660000000000001</v>
       </c>
-      <c r="J48" s="15">
+      <c r="J47" s="15">
         <v>0.88185000000000002</v>
       </c>
-      <c r="K48" s="16">
+      <c r="K47" s="16">
         <f t="shared" si="4"/>
         <v>0.36416772554002541</v>
       </c>
-      <c r="L48" s="15"/>
-      <c r="M48" s="15">
+      <c r="L47" s="15"/>
+      <c r="M47" s="15">
         <v>0.88185000000000002</v>
       </c>
-      <c r="N48" s="15" t="s">
-        <v>21</v>
-      </c>
-      <c r="O48" s="15" t="s">
-        <v>22</v>
-      </c>
-      <c r="P48" s="15" t="s">
-        <v>23</v>
-      </c>
-      <c r="Q48" s="15" t="s">
+      <c r="N47" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="O47" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="P47" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q47" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="R48" s="17" t="s">
+      <c r="R47" s="17" t="s">
         <v>34</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added more historical data (small aircraft) to size initial weight.
</commit_message>
<xml_diff>
--- a/Data/RCAircraftHistoricWeightData.xlsx
+++ b/Data/RCAircraftHistoricWeightData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nathe\Desktop\JZ-WannaBee\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NathenCarey\Desktop\PersonalCode\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44E75050-54F0-4056-85FD-1C8124B2B5A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB1B0E5E-A71B-425F-9FCE-C225B50B157A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Aircraft Data" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="378" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="438" uniqueCount="76">
   <si>
     <t>Source</t>
   </si>
@@ -222,6 +222,48 @@
   </si>
   <si>
     <t>EDA 15</t>
+  </si>
+  <si>
+    <t>Paper</t>
+  </si>
+  <si>
+    <t>Revolution 3D Trainer</t>
+  </si>
+  <si>
+    <t>n/a</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Paper </t>
+  </si>
+  <si>
+    <t>Foamtana</t>
+  </si>
+  <si>
+    <t>Electrify Yak 55M</t>
+  </si>
+  <si>
+    <t>Electrify Extra 330SC</t>
+  </si>
+  <si>
+    <t>Hobbico Superstar EP</t>
+  </si>
+  <si>
+    <t>Extra 330 L</t>
+  </si>
+  <si>
+    <t>Edge 540</t>
+  </si>
+  <si>
+    <t>Carbon Yak 54</t>
+  </si>
+  <si>
+    <t>Hawker Hurricane 25e</t>
+  </si>
+  <si>
+    <t>F3A/Gadfly</t>
+  </si>
+  <si>
+    <t>Nemesis Racer EP</t>
   </si>
 </sst>
 </file>
@@ -231,7 +273,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -242,6 +284,13 @@
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -463,7 +512,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -525,6 +574,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -574,7 +625,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:R47">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:R61">
   <tableColumns count="18">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Source"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Aircraft"/>
@@ -800,15 +851,16 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:R47"/>
+  <dimension ref="A1:T58"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D51" sqref="D51"/>
+      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H72" sqref="H72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
+    <col min="2" max="2" width="17.140625" customWidth="1"/>
     <col min="3" max="3" width="13.7109375" customWidth="1"/>
     <col min="4" max="4" width="14.28515625" customWidth="1"/>
     <col min="5" max="6" width="14.7109375" customWidth="1"/>
@@ -824,7 +876,7 @@
     <col min="18" max="18" width="16.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -880,7 +932,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="18"/>
       <c r="B2" s="19"/>
       <c r="C2" s="19"/>
@@ -900,7 +952,7 @@
       <c r="Q2" s="19"/>
       <c r="R2" s="20"/>
     </row>
-    <row r="3" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>18</v>
       </c>
@@ -956,7 +1008,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="9" t="s">
         <v>18</v>
       </c>
@@ -1012,7 +1064,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
         <v>18</v>
       </c>
@@ -1068,7 +1120,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="9" t="s">
         <v>18</v>
       </c>
@@ -1124,7 +1176,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
         <v>18</v>
       </c>
@@ -1180,7 +1232,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="8" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="9" t="s">
         <v>18</v>
       </c>
@@ -1235,8 +1287,9 @@
       <c r="R8" s="13" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="9" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="T8" s="22"/>
+    </row>
+    <row r="9" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
         <v>18</v>
       </c>
@@ -1292,7 +1345,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="10" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="9" t="s">
         <v>18</v>
       </c>
@@ -1348,7 +1401,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="11" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
         <v>18</v>
       </c>
@@ -1404,7 +1457,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="12" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="9" t="s">
         <v>18</v>
       </c>
@@ -1459,7 +1512,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="13" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
         <v>18</v>
       </c>
@@ -1514,7 +1567,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="14" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="9" t="s">
         <v>18</v>
       </c>
@@ -1569,7 +1622,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="15" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
         <v>18</v>
       </c>
@@ -1624,7 +1677,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="16" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="9" t="s">
         <v>18</v>
       </c>
@@ -2100,7 +2153,7 @@
         <v>1.59</v>
       </c>
       <c r="K24" s="6">
-        <f t="shared" ref="K24:K47" si="4">I24/G24</f>
+        <f t="shared" ref="K24:K58" si="4">I24/G24</f>
         <v>1</v>
       </c>
       <c r="L24" s="5"/>
@@ -3242,13 +3295,13 @@
         <v>1</v>
       </c>
       <c r="G45" s="10">
-        <v>691</v>
+        <v>6.91</v>
       </c>
       <c r="H45" s="10">
         <v>0</v>
       </c>
       <c r="I45" s="10">
-        <v>461</v>
+        <v>4.6100000000000003</v>
       </c>
       <c r="J45" s="10">
         <v>1.5</v>
@@ -3386,6 +3439,417 @@
       </c>
       <c r="R47" s="17" t="s">
         <v>34</v>
+      </c>
+    </row>
+    <row r="48" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A48" s="21" t="s">
+        <v>62</v>
+      </c>
+      <c r="B48" s="21" t="s">
+        <v>63</v>
+      </c>
+      <c r="C48" s="21" t="s">
+        <v>64</v>
+      </c>
+      <c r="D48" s="21" t="s">
+        <v>64</v>
+      </c>
+      <c r="E48" s="21" t="s">
+        <v>64</v>
+      </c>
+      <c r="F48" s="21" t="s">
+        <v>64</v>
+      </c>
+      <c r="G48">
+        <f>0.43*2.20462262</f>
+        <v>0.94798772659999997</v>
+      </c>
+      <c r="H48">
+        <v>0</v>
+      </c>
+      <c r="I48" s="21">
+        <f>0.282*2.20462262</f>
+        <v>0.62170357883999994</v>
+      </c>
+      <c r="J48">
+        <f>0.148*2.20462262</f>
+        <v>0.32628414775999998</v>
+      </c>
+      <c r="K48" s="16">
+        <f t="shared" si="4"/>
+        <v>0.65581395348837201</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A49" s="21" t="s">
+        <v>62</v>
+      </c>
+      <c r="B49" s="21" t="s">
+        <v>66</v>
+      </c>
+      <c r="C49" s="21" t="s">
+        <v>64</v>
+      </c>
+      <c r="D49" s="21" t="s">
+        <v>64</v>
+      </c>
+      <c r="E49" s="21" t="s">
+        <v>64</v>
+      </c>
+      <c r="F49" s="21" t="s">
+        <v>64</v>
+      </c>
+      <c r="G49">
+        <f>0.45*2.20462262</f>
+        <v>0.99208017900000001</v>
+      </c>
+      <c r="H49">
+        <v>0</v>
+      </c>
+      <c r="I49">
+        <f>0.28*2.20462262</f>
+        <v>0.61729433359999997</v>
+      </c>
+      <c r="J49">
+        <f>0.17*2.20462262</f>
+        <v>0.37478584539999998</v>
+      </c>
+      <c r="K49" s="16">
+        <f t="shared" si="4"/>
+        <v>0.62222222222222223</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A50" s="21" t="s">
+        <v>65</v>
+      </c>
+      <c r="B50" s="21" t="s">
+        <v>67</v>
+      </c>
+      <c r="C50" s="21" t="s">
+        <v>64</v>
+      </c>
+      <c r="D50" s="21" t="s">
+        <v>64</v>
+      </c>
+      <c r="E50" s="21" t="s">
+        <v>64</v>
+      </c>
+      <c r="F50" s="21" t="s">
+        <v>64</v>
+      </c>
+      <c r="G50">
+        <f>1.7*2.20462262</f>
+        <v>3.7478584539999997</v>
+      </c>
+      <c r="H50">
+        <v>0</v>
+      </c>
+      <c r="I50">
+        <f>1.187*2.20462262</f>
+        <v>2.6168870499399999</v>
+      </c>
+      <c r="J50">
+        <f>0.513*2.20462262</f>
+        <v>1.1309714040599999</v>
+      </c>
+      <c r="K50" s="16">
+        <f t="shared" si="4"/>
+        <v>0.69823529411764707</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A51" s="21" t="s">
+        <v>65</v>
+      </c>
+      <c r="B51" s="21" t="s">
+        <v>68</v>
+      </c>
+      <c r="C51" s="21" t="s">
+        <v>64</v>
+      </c>
+      <c r="D51" s="21" t="s">
+        <v>64</v>
+      </c>
+      <c r="E51" s="21" t="s">
+        <v>64</v>
+      </c>
+      <c r="F51" s="21" t="s">
+        <v>64</v>
+      </c>
+      <c r="G51">
+        <f>0.234*2.20462262</f>
+        <v>0.51588169307999998</v>
+      </c>
+      <c r="H51">
+        <v>0</v>
+      </c>
+      <c r="I51">
+        <f>0.178*2.20462262</f>
+        <v>0.39242282635999998</v>
+      </c>
+      <c r="J51">
+        <f>0.056*2.20462262</f>
+        <v>0.12345886671999999</v>
+      </c>
+      <c r="K51" s="16">
+        <f t="shared" si="4"/>
+        <v>0.76068376068376065</v>
+      </c>
+    </row>
+    <row r="52" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A52" s="21" t="s">
+        <v>65</v>
+      </c>
+      <c r="B52" s="21" t="s">
+        <v>69</v>
+      </c>
+      <c r="C52" s="21" t="s">
+        <v>64</v>
+      </c>
+      <c r="D52" s="21" t="s">
+        <v>64</v>
+      </c>
+      <c r="E52" s="21" t="s">
+        <v>64</v>
+      </c>
+      <c r="F52" s="21" t="s">
+        <v>64</v>
+      </c>
+      <c r="G52">
+        <f>1.23*2.20462262</f>
+        <v>2.7116858225999998</v>
+      </c>
+      <c r="H52">
+        <v>0</v>
+      </c>
+      <c r="I52">
+        <f>0.918*2.20462262</f>
+        <v>2.02384356516</v>
+      </c>
+      <c r="J52">
+        <f>0.312*2.20462262</f>
+        <v>0.68784225743999994</v>
+      </c>
+      <c r="K52" s="16">
+        <f t="shared" si="4"/>
+        <v>0.74634146341463414</v>
+      </c>
+    </row>
+    <row r="53" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A53" s="21" t="s">
+        <v>65</v>
+      </c>
+      <c r="B53" s="21" t="s">
+        <v>70</v>
+      </c>
+      <c r="D53" s="21" t="s">
+        <v>64</v>
+      </c>
+      <c r="E53" s="21" t="s">
+        <v>64</v>
+      </c>
+      <c r="F53" s="21" t="s">
+        <v>64</v>
+      </c>
+      <c r="G53">
+        <f>0.62*2.20462262</f>
+        <v>1.3668660243999999</v>
+      </c>
+      <c r="H53">
+        <v>0</v>
+      </c>
+      <c r="I53">
+        <f>0.427*2.20462262</f>
+        <v>0.9413738587399999</v>
+      </c>
+      <c r="J53">
+        <f>0.193*2.20462262</f>
+        <v>0.42549216565999998</v>
+      </c>
+      <c r="K53" s="16">
+        <f t="shared" si="4"/>
+        <v>0.68870967741935485</v>
+      </c>
+    </row>
+    <row r="54" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A54" s="21" t="s">
+        <v>62</v>
+      </c>
+      <c r="B54" s="21" t="s">
+        <v>71</v>
+      </c>
+      <c r="D54" s="21" t="s">
+        <v>64</v>
+      </c>
+      <c r="E54" s="21" t="s">
+        <v>64</v>
+      </c>
+      <c r="F54" s="21" t="s">
+        <v>64</v>
+      </c>
+      <c r="G54">
+        <f>1.65*2.20462262</f>
+        <v>3.6376273229999998</v>
+      </c>
+      <c r="H54">
+        <v>0</v>
+      </c>
+      <c r="I54">
+        <f>1.157*2.20462262</f>
+        <v>2.5507483713400001</v>
+      </c>
+      <c r="J54">
+        <f>0.493*2.20462262</f>
+        <v>1.0868789516599999</v>
+      </c>
+      <c r="K54" s="16">
+        <f t="shared" si="4"/>
+        <v>0.70121212121212129</v>
+      </c>
+    </row>
+    <row r="55" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A55" s="21" t="s">
+        <v>62</v>
+      </c>
+      <c r="B55" s="21" t="s">
+        <v>72</v>
+      </c>
+      <c r="D55" s="21" t="s">
+        <v>64</v>
+      </c>
+      <c r="E55" s="21" t="s">
+        <v>64</v>
+      </c>
+      <c r="F55" s="21" t="s">
+        <v>64</v>
+      </c>
+      <c r="G55">
+        <f>1.73*2.20462262</f>
+        <v>3.8139971326</v>
+      </c>
+      <c r="H55">
+        <v>0</v>
+      </c>
+      <c r="I55">
+        <f>1.139*2.20462262</f>
+        <v>2.5110651641799997</v>
+      </c>
+      <c r="J55">
+        <f>0.591*2.20462262</f>
+        <v>1.3029319684199998</v>
+      </c>
+      <c r="K55" s="16">
+        <f t="shared" si="4"/>
+        <v>0.65838150289017339</v>
+      </c>
+    </row>
+    <row r="56" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A56" s="21" t="s">
+        <v>62</v>
+      </c>
+      <c r="B56" s="21" t="s">
+        <v>73</v>
+      </c>
+      <c r="D56" s="21" t="s">
+        <v>64</v>
+      </c>
+      <c r="E56" s="21" t="s">
+        <v>64</v>
+      </c>
+      <c r="F56" s="21" t="s">
+        <v>64</v>
+      </c>
+      <c r="G56">
+        <f>2.1*2.20462262</f>
+        <v>4.6297075019999996</v>
+      </c>
+      <c r="H56">
+        <v>0</v>
+      </c>
+      <c r="I56">
+        <f>1.528*2.20462262</f>
+        <v>3.3686633633600001</v>
+      </c>
+      <c r="J56">
+        <f>0.572*2.20462262</f>
+        <v>1.2610441386399998</v>
+      </c>
+      <c r="K56" s="16">
+        <f t="shared" si="4"/>
+        <v>0.72761904761904772</v>
+      </c>
+    </row>
+    <row r="57" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A57" s="21" t="s">
+        <v>62</v>
+      </c>
+      <c r="B57" s="21" t="s">
+        <v>74</v>
+      </c>
+      <c r="D57" s="21" t="s">
+        <v>64</v>
+      </c>
+      <c r="E57" s="21" t="s">
+        <v>64</v>
+      </c>
+      <c r="F57" s="21" t="s">
+        <v>64</v>
+      </c>
+      <c r="G57">
+        <f>2.35*2.20462262</f>
+        <v>5.1808631570000001</v>
+      </c>
+      <c r="H57">
+        <v>0</v>
+      </c>
+      <c r="I57">
+        <f>1.713*2.20462262</f>
+        <v>3.7765185480599999</v>
+      </c>
+      <c r="J57">
+        <f>0.637*2.20462262</f>
+        <v>1.40434460894</v>
+      </c>
+      <c r="K57" s="16">
+        <f t="shared" si="4"/>
+        <v>0.72893617021276591</v>
+      </c>
+    </row>
+    <row r="58" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A58" s="21" t="s">
+        <v>62</v>
+      </c>
+      <c r="B58" s="21" t="s">
+        <v>75</v>
+      </c>
+      <c r="D58" s="21" t="s">
+        <v>64</v>
+      </c>
+      <c r="E58" s="21" t="s">
+        <v>64</v>
+      </c>
+      <c r="F58" s="21" t="s">
+        <v>64</v>
+      </c>
+      <c r="G58">
+        <f>2.1*2.20462262</f>
+        <v>4.6297075019999996</v>
+      </c>
+      <c r="H58">
+        <v>0</v>
+      </c>
+      <c r="I58">
+        <f>1.139*2.20462262</f>
+        <v>2.5110651641799997</v>
+      </c>
+      <c r="J58">
+        <f>0.71*2.20462262</f>
+        <v>1.5652820601999999</v>
+      </c>
+      <c r="K58" s="16">
+        <f t="shared" si="4"/>
+        <v>0.54238095238095241</v>
       </c>
     </row>
   </sheetData>

</xml_diff>